<commit_message>
Updated membership setup tests
</commit_message>
<xml_diff>
--- a/Membership/Create Benefit/Main.rvl.xlsx
+++ b/Membership/Create Benefit/Main.rvl.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3064" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3179" uniqueCount="217">
   <si>
     <t>Flow</t>
   </si>
@@ -597,6 +597,78 @@
   <si>
     <t>C:\UX 365 Regression Testing\JSON\Global.json</t>
   </si>
+  <si>
+    <t>\MembershipData.xls</t>
+  </si>
+  <si>
+    <t>***Test creates all Installments in MembershipData spreadsheet.</t>
+  </si>
+  <si>
+    <t>****Test first searches for the installment to see if it already exists.</t>
+  </si>
+  <si>
+    <t>*****If it already exists, the installment is not created.</t>
+  </si>
+  <si>
+    <t>******If it doesn't exist, the test creates the installment using the data in the spreadsheet.</t>
+  </si>
+  <si>
+    <t>DoLoadObjects</t>
+  </si>
+  <si>
+    <t>objectsFilePath</t>
+  </si>
+  <si>
+    <t>C:\UX365RegressionTest\Objects.js</t>
+  </si>
+  <si>
+    <t>***Test creates all Benefits in MembershipData spreadsheet.</t>
+  </si>
+  <si>
+    <t>****Test first searches for the benefit to see if it already exists.</t>
+  </si>
+  <si>
+    <t>*****If it already exists, the benefit is not created.</t>
+  </si>
+  <si>
+    <t>******If it doesn't exist, the test creates the benefit using the data in the spreadsheet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benefit: </t>
+  </si>
+  <si>
+    <t>C:\UX365RegressionTest\JSON\Global.json</t>
+  </si>
+  <si>
+    <t>*******After each benefit is created, the Create Rate test run to create all of the rates for that benefit.</t>
+  </si>
+  <si>
+    <t>Test sets value for BenefitName in global JSON, so Create Rate test knows which benefit to use.</t>
+  </si>
+  <si>
+    <t>UX_Grid</t>
+  </si>
+  <si>
+    <t>Benefit not found. Create Benefit.</t>
+  </si>
+  <si>
+    <t>If a Calendar membership, set the Prorate and Prorate Cycle fields.</t>
+  </si>
+  <si>
+    <t>If the benefit is a Calendar membership, set the Prorate and Prorate Cycle fields.</t>
+  </si>
+  <si>
+    <t>*****Run Create Rate test to create the rates for this benefit.</t>
+  </si>
+  <si>
+    <t>*****Run Create Rate test to create the rates for this benefit.*****</t>
+  </si>
+  <si>
+    <t>C:\UX365RegressionTest\Membership\MembershipData.xls</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
 </sst>
 </file>
 
@@ -616,7 +688,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7982">
+  <borders count="8000">
     <border>
       <left/>
       <right/>
@@ -8605,11 +8677,29 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7982">
+  <cellXfs count="8000">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -16592,6 +16682,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7979" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7980" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7981" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7982" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7983" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7984" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7985" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7986" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7987" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7988" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7989" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7990" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7991" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7992" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7993" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7994" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7995" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7996" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7997" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7998" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7999" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16601,7 +16709,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H90"/>
+  <dimension ref="A1:H104"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.5546875" customWidth="true"/>
@@ -16687,7 +16795,7 @@
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6">
@@ -16774,288 +16882,266 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2944"/>
+      <c r="A12" s="7989"/>
     </row>
     <row r="13">
-      <c r="A13" s="2943" t="s">
-        <v>29</v>
-      </c>
+      <c r="A13" s="7987"/>
       <c r="B13" t="s">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>144</v>
+        <v>44</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="F13" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="G13" t="s">
-        <v>54</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2942"/>
+      <c r="A14" s="7986"/>
       <c r="B14" t="s">
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="F14" t="s">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>63</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2941"/>
+      <c r="A15" s="7985"/>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="2940" t="s">
-        <v>31</v>
-      </c>
+      <c r="A16" s="7984"/>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>153</v>
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2939" t="s">
-        <v>29</v>
-      </c>
+      <c r="A17" s="7992"/>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2938" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" t="s">
-        <v>64</v>
-      </c>
+      <c r="A18" s="7983"/>
     </row>
     <row r="19">
-      <c r="A19" s="2937"/>
+      <c r="A19" s="7982"/>
       <c r="B19" t="s">
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>44</v>
+        <v>198</v>
       </c>
       <c r="E19" t="s">
-        <v>45</v>
+        <v>199</v>
       </c>
       <c r="F19" t="s">
         <v>10</v>
       </c>
       <c r="G19" t="s">
-        <v>65</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="2936"/>
-      <c r="B20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" t="s">
-        <v>68</v>
-      </c>
-      <c r="F20" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" t="s">
-        <v>69</v>
-      </c>
+      <c r="A20" s="2944"/>
     </row>
     <row r="21">
-      <c r="A21" s="2935"/>
+      <c r="A21" s="2943" t="s">
+        <v>29</v>
+      </c>
       <c r="B21" t="s">
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
-        <v>70</v>
+        <v>144</v>
       </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="F21" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="G21" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="2934"/>
+      <c r="A22" s="2942"/>
       <c r="B22" t="s">
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D22" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E22" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="F22" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="G22" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="2933" t="s">
+      <c r="A23" s="2941"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="2940" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2939" t="s">
         <v>29</v>
       </c>
-      <c r="B23" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="2932"/>
-      <c r="B24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" t="s">
-        <v>169</v>
-      </c>
-      <c r="E24" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="2931"/>
       <c r="B25" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" t="s">
-        <v>75</v>
-      </c>
-      <c r="F25" t="s">
-        <v>153</v>
-      </c>
-      <c r="G25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="2930"/>
+      <c r="A26" s="2938" t="s">
+        <v>29</v>
+      </c>
       <c r="B26" t="s">
-        <v>17</v>
-      </c>
-      <c r="E26" t="s">
-        <v>171</v>
-      </c>
-      <c r="F26" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26" t="s">
-        <v>192</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="2929" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" t="s">
-        <v>180</v>
-      </c>
+      <c r="A27" s="7998"/>
     </row>
     <row r="28">
-      <c r="A28" s="2928"/>
+      <c r="A28" s="2937"/>
       <c r="B28" t="s">
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="D28" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="E28" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="F28" t="s">
-        <v>153</v>
+        <v>10</v>
       </c>
       <c r="G28" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="2927"/>
+      <c r="A29" s="7990"/>
       <c r="B29" t="s">
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D29" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="E29" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="F29" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="G29" t="s">
-        <v>79</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="2926"/>
+      <c r="A30" s="7991"/>
       <c r="B30" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" t="s">
-        <v>80</v>
-      </c>
-      <c r="D30" t="s">
-        <v>131</v>
+        <v>17</v>
       </c>
       <c r="E30" t="s">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="F30" t="s">
         <v>153</v>
@@ -17063,111 +17149,160 @@
       <c r="G30" t="s">
         <v>35</v>
       </c>
-      <c r="H30" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="31">
-      <c r="A31" s="2925"/>
+      <c r="A31" s="2936"/>
       <c r="B31" t="s">
-        <v>17</v>
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" t="s">
+        <v>67</v>
       </c>
       <c r="E31" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="F31" t="s">
         <v>10</v>
       </c>
       <c r="G31" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="2924"/>
+      <c r="A32" s="2935"/>
       <c r="B32" t="s">
-        <v>17</v>
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" t="s">
+        <v>70</v>
       </c>
       <c r="E32" t="s">
-        <v>147</v>
+        <v>71</v>
       </c>
       <c r="F32" t="s">
         <v>10</v>
       </c>
       <c r="G32" t="s">
-        <v>149</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="2923" t="s">
-        <v>33</v>
-      </c>
+      <c r="A33" s="2934"/>
       <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" t="s">
+        <v>72</v>
+      </c>
+      <c r="E33" t="s">
+        <v>68</v>
+      </c>
+      <c r="F33" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2933" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="7993"/>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" t="s">
+        <v>45</v>
+      </c>
+      <c r="F35" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2932"/>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" t="s">
+        <v>169</v>
+      </c>
+      <c r="E36" t="s">
+        <v>68</v>
+      </c>
+      <c r="F36" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2931"/>
+      <c r="B37" t="s">
         <v>17</v>
       </c>
-      <c r="E33" t="s">
-        <v>34</v>
-      </c>
-      <c r="F33" t="s">
-        <v>39</v>
-      </c>
-      <c r="G33" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="2922"/>
-      <c r="B34" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="2921"/>
-    </row>
-    <row r="36">
-      <c r="A36" s="2920" t="s">
+      <c r="E37" t="s">
+        <v>75</v>
+      </c>
+      <c r="F37" t="s">
+        <v>153</v>
+      </c>
+      <c r="G37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2930"/>
+      <c r="B38" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" t="s">
+        <v>171</v>
+      </c>
+      <c r="F38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2929" t="s">
         <v>29</v>
       </c>
-      <c r="B36" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="2919"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="2918" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="2917"/>
       <c r="B39" t="s">
-        <v>3</v>
-      </c>
-      <c r="C39" t="s">
-        <v>43</v>
-      </c>
-      <c r="D39" t="s">
-        <v>44</v>
-      </c>
-      <c r="E39" t="s">
-        <v>45</v>
-      </c>
-      <c r="F39" t="s">
-        <v>10</v>
-      </c>
-      <c r="G39" t="s">
-        <v>92</v>
+        <v>180</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="2916"/>
+      <c r="A40" s="2928"/>
       <c r="B40" t="s">
         <v>3</v>
       </c>
@@ -17175,253 +17310,200 @@
         <v>66</v>
       </c>
       <c r="D40" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E40" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="F40" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="G40" t="s">
-        <v>73</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="2915"/>
+      <c r="A41" s="2927"/>
       <c r="B41" t="s">
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D41" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="E41" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="F41" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="G41" t="s">
-        <v>73</v>
+        <v>216</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="2914"/>
+      <c r="A42" s="2926"/>
       <c r="B42" t="s">
         <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>66</v>
+        <v>209</v>
       </c>
       <c r="D42" t="s">
-        <v>94</v>
+        <v>131</v>
       </c>
       <c r="E42" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="F42" t="s">
-        <v>62</v>
+        <v>153</v>
       </c>
       <c r="G42" t="s">
-        <v>96</v>
+        <v>35</v>
+      </c>
+      <c r="H42" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="2913"/>
+      <c r="A43" s="2925"/>
       <c r="B43" t="s">
         <v>17</v>
       </c>
       <c r="E43" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="F43" t="s">
-        <v>153</v>
+        <v>10</v>
       </c>
       <c r="G43" t="s">
-        <v>133</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="2912"/>
+      <c r="A44" s="2924"/>
       <c r="B44" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" t="s">
-        <v>66</v>
-      </c>
-      <c r="D44" t="s">
-        <v>98</v>
+        <v>17</v>
       </c>
       <c r="E44" t="s">
-        <v>95</v>
+        <v>147</v>
       </c>
       <c r="F44" t="s">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="G44" t="s">
-        <v>99</v>
+        <v>149</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="2911"/>
+      <c r="A45" s="2923" t="s">
+        <v>33</v>
+      </c>
       <c r="B45" t="s">
         <v>17</v>
       </c>
       <c r="E45" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="F45" t="s">
-        <v>153</v>
+        <v>39</v>
       </c>
       <c r="G45" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="2910"/>
+      <c r="A46" s="2922"/>
       <c r="B46" t="s">
+        <v>36</v>
+      </c>
+      <c r="D46" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2921"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="2920" t="s">
+        <v>29</v>
+      </c>
+      <c r="B48" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2919"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="2918" t="s">
+        <v>29</v>
+      </c>
+      <c r="B50" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2917"/>
+      <c r="B51" t="s">
         <v>3</v>
       </c>
-      <c r="C46" t="s">
-        <v>66</v>
-      </c>
-      <c r="D46" t="s">
-        <v>94</v>
-      </c>
-      <c r="E46" t="s">
-        <v>95</v>
-      </c>
-      <c r="F46" t="s">
-        <v>62</v>
-      </c>
-      <c r="G46" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="2909"/>
-      <c r="B47" t="s">
-        <v>17</v>
-      </c>
-      <c r="E47" t="s">
-        <v>75</v>
-      </c>
-      <c r="F47" t="s">
-        <v>153</v>
-      </c>
-      <c r="G47" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="2908"/>
-      <c r="B48" t="s">
+      <c r="C51" t="s">
+        <v>43</v>
+      </c>
+      <c r="D51" t="s">
+        <v>44</v>
+      </c>
+      <c r="E51" t="s">
+        <v>45</v>
+      </c>
+      <c r="F51" t="s">
+        <v>10</v>
+      </c>
+      <c r="G51" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="7995"/>
+      <c r="B52" t="s">
         <v>3</v>
       </c>
-      <c r="C48" t="s">
-        <v>102</v>
-      </c>
-      <c r="D48" t="s">
-        <v>103</v>
-      </c>
-      <c r="E48" t="s">
-        <v>104</v>
-      </c>
-      <c r="F48" t="s">
-        <v>153</v>
-      </c>
-      <c r="G48" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="2907"/>
-      <c r="B49" t="s">
-        <v>3</v>
-      </c>
-      <c r="C49" t="s">
-        <v>106</v>
-      </c>
-      <c r="D49" t="s">
-        <v>103</v>
-      </c>
-      <c r="E49" t="s">
-        <v>104</v>
-      </c>
-      <c r="F49" t="s">
-        <v>153</v>
-      </c>
-      <c r="G49" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="2906"/>
-      <c r="B50" t="s">
-        <v>3</v>
-      </c>
-      <c r="C50" t="s">
-        <v>108</v>
-      </c>
-      <c r="D50" t="s">
-        <v>103</v>
-      </c>
-      <c r="E50" t="s">
-        <v>104</v>
-      </c>
-      <c r="F50" t="s">
-        <v>153</v>
-      </c>
-      <c r="G50" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="2905" t="s">
-        <v>33</v>
-      </c>
-      <c r="B51" t="s">
-        <v>17</v>
-      </c>
-      <c r="E51" t="s">
-        <v>34</v>
-      </c>
-      <c r="F51" t="s">
-        <v>153</v>
-      </c>
-      <c r="G51" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="2904"/>
-      <c r="B52" t="s">
-        <v>36</v>
+      <c r="C52" t="s">
+        <v>43</v>
       </c>
       <c r="D52" t="s">
-        <v>37</v>
+        <v>44</v>
+      </c>
+      <c r="E52" t="s">
+        <v>45</v>
+      </c>
+      <c r="F52" t="s">
+        <v>10</v>
+      </c>
+      <c r="G52" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="2903"/>
+      <c r="A53" s="7994"/>
       <c r="B53" t="s">
         <v>17</v>
       </c>
       <c r="E53" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F53" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="G53" t="s">
-        <v>105</v>
+        <v>35</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="2902"/>
+      <c r="A54" s="2916"/>
       <c r="B54" t="s">
         <v>3</v>
       </c>
@@ -17429,61 +17511,77 @@
         <v>66</v>
       </c>
       <c r="D54" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="E54" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="F54" t="s">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="G54" t="s">
-        <v>110</v>
+        <v>73</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="2901"/>
+      <c r="A55" s="2915"/>
       <c r="B55" t="s">
-        <v>17</v>
+        <v>3</v>
+      </c>
+      <c r="C55" t="s">
+        <v>66</v>
+      </c>
+      <c r="D55" t="s">
+        <v>93</v>
       </c>
       <c r="E55" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F55" t="s">
-        <v>153</v>
+        <v>10</v>
       </c>
       <c r="G55" t="s">
-        <v>137</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="2900"/>
+      <c r="A56" s="2914"/>
       <c r="B56" t="s">
         <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>112</v>
+        <v>66</v>
       </c>
       <c r="D56" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="E56" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="F56" t="s">
+        <v>62</v>
+      </c>
+      <c r="G56" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2913"/>
+      <c r="B57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E57" t="s">
+        <v>75</v>
+      </c>
+      <c r="F57" t="s">
         <v>153</v>
       </c>
-      <c r="G56" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="2899" t="s">
-        <v>27</v>
+      <c r="G57" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="2898"/>
+      <c r="A58" s="2912"/>
       <c r="B58" t="s">
         <v>3</v>
       </c>
@@ -17500,11 +17598,11 @@
         <v>62</v>
       </c>
       <c r="G58" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="2897"/>
+      <c r="A59" s="2911"/>
       <c r="B59" t="s">
         <v>17</v>
       </c>
@@ -17515,11 +17613,11 @@
         <v>153</v>
       </c>
       <c r="G59" t="s">
-        <v>139</v>
+        <v>35</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="2896"/>
+      <c r="A60" s="2910"/>
       <c r="B60" t="s">
         <v>3</v>
       </c>
@@ -17527,367 +17625,617 @@
         <v>66</v>
       </c>
       <c r="D60" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="E60" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="F60" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="G60" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="2895"/>
+      <c r="A61" s="2909"/>
       <c r="B61" t="s">
+        <v>17</v>
+      </c>
+      <c r="E61" t="s">
+        <v>75</v>
+      </c>
+      <c r="F61" t="s">
+        <v>153</v>
+      </c>
+      <c r="G61" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2908"/>
+      <c r="B62" t="s">
         <v>3</v>
       </c>
-      <c r="C61" t="s">
-        <v>66</v>
-      </c>
-      <c r="D61" t="s">
-        <v>119</v>
-      </c>
-      <c r="E61" t="s">
-        <v>95</v>
-      </c>
-      <c r="F61" t="s">
-        <v>62</v>
-      </c>
-      <c r="G61" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="2894"/>
-      <c r="B62" t="s">
-        <v>17</v>
+      <c r="C62" t="s">
+        <v>102</v>
+      </c>
+      <c r="D62" t="s">
+        <v>103</v>
       </c>
       <c r="E62" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="F62" t="s">
         <v>153</v>
       </c>
       <c r="G62" t="s">
-        <v>140</v>
+        <v>51</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="2893"/>
+      <c r="A63" s="2907"/>
       <c r="B63" t="s">
         <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="D63" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="E63" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="F63" t="s">
-        <v>62</v>
+        <v>153</v>
       </c>
       <c r="G63" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="2892"/>
+      <c r="A64" s="2906"/>
       <c r="B64" t="s">
-        <v>17</v>
+        <v>3</v>
+      </c>
+      <c r="C64" t="s">
+        <v>108</v>
+      </c>
+      <c r="D64" t="s">
+        <v>103</v>
       </c>
       <c r="E64" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="F64" t="s">
         <v>153</v>
       </c>
       <c r="G64" t="s">
-        <v>141</v>
+        <v>52</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="2891"/>
+      <c r="A65" s="7996"/>
       <c r="B65" t="s">
         <v>3</v>
       </c>
       <c r="C65" t="s">
+        <v>43</v>
+      </c>
+      <c r="D65" t="s">
+        <v>44</v>
+      </c>
+      <c r="E65" t="s">
+        <v>45</v>
+      </c>
+      <c r="F65" t="s">
+        <v>10</v>
+      </c>
+      <c r="G65" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2905" t="s">
+        <v>33</v>
+      </c>
+      <c r="B66" t="s">
+        <v>17</v>
+      </c>
+      <c r="E66" t="s">
+        <v>34</v>
+      </c>
+      <c r="F66" t="s">
+        <v>153</v>
+      </c>
+      <c r="G66" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2904"/>
+      <c r="B67" t="s">
+        <v>36</v>
+      </c>
+      <c r="D67" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2903"/>
+      <c r="B68" t="s">
+        <v>17</v>
+      </c>
+      <c r="E68" t="s">
+        <v>38</v>
+      </c>
+      <c r="F68" t="s">
+        <v>10</v>
+      </c>
+      <c r="G68" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2902"/>
+      <c r="B69" t="s">
+        <v>3</v>
+      </c>
+      <c r="C69" t="s">
         <v>66</v>
       </c>
-      <c r="D65" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="2890"/>
-      <c r="B66" t="s">
-        <v>3</v>
-      </c>
-      <c r="C66" t="s">
-        <v>53</v>
-      </c>
-      <c r="D66" t="s">
-        <v>77</v>
-      </c>
-      <c r="E66" t="s">
-        <v>78</v>
-      </c>
-      <c r="F66" t="s">
-        <v>21</v>
-      </c>
-      <c r="G66" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="2889"/>
-      <c r="B67" t="s">
-        <v>3</v>
-      </c>
-      <c r="C67" t="s">
-        <v>43</v>
-      </c>
-      <c r="D67" t="s">
-        <v>44</v>
-      </c>
-      <c r="E67" t="s">
-        <v>45</v>
-      </c>
-      <c r="F67" t="s">
-        <v>10</v>
-      </c>
-      <c r="G67" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="2888"/>
-      <c r="B68" t="s">
-        <v>3</v>
-      </c>
-      <c r="C68" t="s">
-        <v>66</v>
-      </c>
-      <c r="D68" t="s">
-        <v>126</v>
-      </c>
-      <c r="E68" t="s">
+      <c r="D69" t="s">
+        <v>94</v>
+      </c>
+      <c r="E69" t="s">
         <v>95</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F69" t="s">
         <v>62</v>
       </c>
-      <c r="G68" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="2887"/>
-      <c r="B69" t="s">
-        <v>17</v>
-      </c>
-      <c r="E69" t="s">
-        <v>128</v>
-      </c>
-      <c r="F69" t="s">
-        <v>153</v>
-      </c>
       <c r="G69" t="s">
-        <v>35</v>
+        <v>110</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="2886"/>
+      <c r="A70" s="2901"/>
       <c r="B70" t="s">
         <v>17</v>
       </c>
       <c r="E70" t="s">
-        <v>130</v>
+        <v>75</v>
       </c>
       <c r="F70" t="s">
         <v>153</v>
       </c>
       <c r="G70" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2900"/>
+      <c r="B71" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71" t="s">
+        <v>112</v>
+      </c>
+      <c r="D71" t="s">
+        <v>103</v>
+      </c>
+      <c r="E71" t="s">
+        <v>104</v>
+      </c>
+      <c r="F71" t="s">
+        <v>153</v>
+      </c>
+      <c r="G71" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2899" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2898"/>
+      <c r="B73" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73" t="s">
+        <v>66</v>
+      </c>
+      <c r="D73" t="s">
+        <v>98</v>
+      </c>
+      <c r="E73" t="s">
+        <v>95</v>
+      </c>
+      <c r="F73" t="s">
+        <v>62</v>
+      </c>
+      <c r="G73" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2897"/>
+      <c r="B74" t="s">
+        <v>17</v>
+      </c>
+      <c r="E74" t="s">
+        <v>75</v>
+      </c>
+      <c r="F74" t="s">
+        <v>153</v>
+      </c>
+      <c r="G74" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="2896"/>
+      <c r="B75" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75" t="s">
+        <v>66</v>
+      </c>
+      <c r="D75" t="s">
+        <v>116</v>
+      </c>
+      <c r="E75" t="s">
+        <v>117</v>
+      </c>
+      <c r="F75" t="s">
+        <v>10</v>
+      </c>
+      <c r="G75" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2895"/>
+      <c r="B76" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76" t="s">
+        <v>66</v>
+      </c>
+      <c r="D76" t="s">
+        <v>119</v>
+      </c>
+      <c r="E76" t="s">
+        <v>95</v>
+      </c>
+      <c r="F76" t="s">
+        <v>62</v>
+      </c>
+      <c r="G76" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="2894"/>
+      <c r="B77" t="s">
+        <v>17</v>
+      </c>
+      <c r="E77" t="s">
+        <v>75</v>
+      </c>
+      <c r="F77" t="s">
+        <v>153</v>
+      </c>
+      <c r="G77" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="2893"/>
+      <c r="B78" t="s">
+        <v>3</v>
+      </c>
+      <c r="C78" t="s">
+        <v>66</v>
+      </c>
+      <c r="D78" t="s">
+        <v>119</v>
+      </c>
+      <c r="E78" t="s">
+        <v>95</v>
+      </c>
+      <c r="F78" t="s">
+        <v>62</v>
+      </c>
+      <c r="G78" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="2892"/>
+      <c r="B79" t="s">
+        <v>17</v>
+      </c>
+      <c r="E79" t="s">
+        <v>75</v>
+      </c>
+      <c r="F79" t="s">
+        <v>153</v>
+      </c>
+      <c r="G79" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2891"/>
+      <c r="B80" t="s">
+        <v>3</v>
+      </c>
+      <c r="C80" t="s">
+        <v>66</v>
+      </c>
+      <c r="D80" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="2890"/>
+      <c r="B81" t="s">
+        <v>3</v>
+      </c>
+      <c r="C81" t="s">
+        <v>53</v>
+      </c>
+      <c r="D81" t="s">
+        <v>77</v>
+      </c>
+      <c r="E81" t="s">
+        <v>78</v>
+      </c>
+      <c r="F81" t="s">
+        <v>21</v>
+      </c>
+      <c r="G81" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2889"/>
+      <c r="B82" t="s">
+        <v>3</v>
+      </c>
+      <c r="C82" t="s">
+        <v>43</v>
+      </c>
+      <c r="D82" t="s">
+        <v>44</v>
+      </c>
+      <c r="E82" t="s">
+        <v>45</v>
+      </c>
+      <c r="F82" t="s">
+        <v>10</v>
+      </c>
+      <c r="G82" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="2888"/>
+      <c r="B83" t="s">
+        <v>3</v>
+      </c>
+      <c r="C83" t="s">
+        <v>66</v>
+      </c>
+      <c r="D83" t="s">
+        <v>126</v>
+      </c>
+      <c r="E83" t="s">
+        <v>130</v>
+      </c>
+      <c r="F83" t="s">
+        <v>153</v>
+      </c>
+      <c r="G83" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="71">
-      <c r="A71" s="2885"/>
-    </row>
-    <row r="72">
-      <c r="A72" s="2884"/>
-    </row>
-    <row r="73">
-      <c r="A73" s="2883" t="s">
+    <row r="84">
+      <c r="A84" s="2885"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="2884"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="2883" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" s="2882"/>
-      <c r="B74" t="s">
+    <row r="87">
+      <c r="A87" s="7997"/>
+      <c r="B87" t="s">
         <v>3</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C87" t="s">
+        <v>43</v>
+      </c>
+      <c r="D87" t="s">
+        <v>44</v>
+      </c>
+      <c r="E87" t="s">
+        <v>45</v>
+      </c>
+      <c r="F87" t="s">
+        <v>10</v>
+      </c>
+      <c r="G87" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2882"/>
+      <c r="B88" t="s">
+        <v>3</v>
+      </c>
+      <c r="C88" t="s">
         <v>181</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D88" t="s">
         <v>182</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E88" t="s">
         <v>183</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F88" t="s">
         <v>10</v>
       </c>
-      <c r="G74" t="s">
+      <c r="G88" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="75">
-      <c r="A75" s="2881"/>
-    </row>
-    <row r="76">
-      <c r="A76" s="2880" t="s">
+    <row r="89">
+      <c r="A89" s="2881"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="2880" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="77">
-      <c r="A77" s="2879"/>
-    </row>
-    <row r="78">
-      <c r="A78" s="57"/>
-      <c r="B78" s="58"/>
-      <c r="C78" s="59"/>
-      <c r="D78" s="60"/>
-      <c r="E78" s="61"/>
-      <c r="F78" s="62"/>
-      <c r="G78" s="63"/>
-      <c r="H78" s="64"/>
-    </row>
-    <row r="79">
-      <c r="A79" s="65"/>
-      <c r="B79" s="66"/>
-      <c r="C79" s="67"/>
-      <c r="D79" s="68"/>
-      <c r="E79" s="69"/>
-      <c r="F79" s="70"/>
-      <c r="G79" s="71"/>
-      <c r="H79" s="72"/>
-    </row>
-    <row r="80">
-      <c r="A80" s="73"/>
-      <c r="B80" s="74"/>
-      <c r="C80" s="75"/>
-      <c r="D80" s="76"/>
-      <c r="E80" s="77"/>
-      <c r="F80" s="78"/>
-      <c r="G80" s="79"/>
-      <c r="H80" s="80"/>
-    </row>
-    <row r="81">
-      <c r="A81" s="81"/>
-      <c r="B81" s="82"/>
-      <c r="C81" s="83"/>
-      <c r="D81" s="84"/>
-      <c r="E81" s="85"/>
-      <c r="F81" s="86"/>
-      <c r="G81" s="87"/>
-      <c r="H81" s="88"/>
-    </row>
-    <row r="82">
-      <c r="A82" s="89"/>
-      <c r="B82" s="90"/>
-      <c r="C82" s="91"/>
-      <c r="D82" s="92"/>
-      <c r="E82" s="93"/>
-      <c r="F82" s="94"/>
-      <c r="G82" s="95"/>
-      <c r="H82" s="96"/>
-    </row>
-    <row r="83">
-      <c r="A83" s="97"/>
-      <c r="B83" s="98"/>
-      <c r="C83" s="99"/>
-      <c r="D83" s="100"/>
-      <c r="E83" s="101"/>
-      <c r="F83" s="102"/>
-      <c r="G83" s="103"/>
-      <c r="H83" s="104"/>
-    </row>
-    <row r="84">
-      <c r="A84" s="105"/>
-      <c r="B84" s="106"/>
-      <c r="C84" s="107"/>
-      <c r="D84" s="108"/>
-      <c r="E84" s="109"/>
-      <c r="F84" s="110"/>
-      <c r="G84" s="111"/>
-      <c r="H84" s="112"/>
-    </row>
-    <row r="85">
-      <c r="A85" s="113"/>
-      <c r="B85" s="114"/>
-      <c r="C85" s="115"/>
-      <c r="D85" s="116"/>
-      <c r="E85" s="117"/>
-      <c r="F85" s="118"/>
-      <c r="G85" s="119"/>
-      <c r="H85" s="120"/>
-    </row>
-    <row r="86">
-      <c r="A86" s="121"/>
-      <c r="B86" s="122"/>
-      <c r="C86" s="123"/>
-      <c r="D86" s="124"/>
-      <c r="E86" s="125"/>
-      <c r="F86" s="126"/>
-      <c r="G86" s="127"/>
-      <c r="H86" s="128"/>
-    </row>
-    <row r="87">
-      <c r="A87" s="129"/>
-      <c r="B87" s="130"/>
-      <c r="C87" s="131"/>
-      <c r="D87" s="132"/>
-      <c r="E87" s="133"/>
-      <c r="F87" s="134"/>
-      <c r="G87" s="135"/>
-      <c r="H87" s="136"/>
-    </row>
-    <row r="88">
-      <c r="A88" s="137"/>
-      <c r="B88" s="138"/>
-      <c r="C88" s="139"/>
-      <c r="D88" s="140"/>
-      <c r="E88" s="141"/>
-      <c r="F88" s="142"/>
-      <c r="G88" s="143"/>
-      <c r="H88" s="144"/>
-    </row>
-    <row r="89">
-      <c r="A89" s="145"/>
-      <c r="B89" s="146"/>
-      <c r="C89" s="147"/>
-      <c r="D89" s="148"/>
-      <c r="E89" s="149"/>
-      <c r="F89" s="150"/>
-      <c r="G89" s="151"/>
-      <c r="H89" s="152"/>
-    </row>
-    <row r="90">
-      <c r="A90" s="153"/>
-      <c r="B90" s="154"/>
-      <c r="C90" s="155"/>
-      <c r="D90" s="156"/>
-      <c r="E90" s="157"/>
-      <c r="F90" s="158"/>
-      <c r="G90" s="159"/>
-      <c r="H90" s="160"/>
+    <row r="91">
+      <c r="A91" s="2879"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="57"/>
+      <c r="B92" s="58"/>
+      <c r="C92" s="59"/>
+      <c r="D92" s="60"/>
+      <c r="E92" s="61"/>
+      <c r="F92" s="62"/>
+      <c r="G92" s="63"/>
+      <c r="H92" s="64"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="65"/>
+      <c r="B93" s="66"/>
+      <c r="C93" s="67"/>
+      <c r="D93" s="68"/>
+      <c r="E93" s="69"/>
+      <c r="F93" s="70"/>
+      <c r="G93" s="71"/>
+      <c r="H93" s="72"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="73"/>
+      <c r="B94" s="74"/>
+      <c r="C94" s="75"/>
+      <c r="D94" s="76"/>
+      <c r="E94" s="77"/>
+      <c r="F94" s="78"/>
+      <c r="G94" s="79"/>
+      <c r="H94" s="80"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="81"/>
+      <c r="B95" s="82"/>
+      <c r="C95" s="83"/>
+      <c r="D95" s="84"/>
+      <c r="E95" s="85"/>
+      <c r="F95" s="86"/>
+      <c r="G95" s="87"/>
+      <c r="H95" s="88"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="89"/>
+      <c r="B96" s="90"/>
+      <c r="C96" s="91"/>
+      <c r="D96" s="92"/>
+      <c r="E96" s="93"/>
+      <c r="F96" s="94"/>
+      <c r="G96" s="95"/>
+      <c r="H96" s="96"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="97"/>
+      <c r="B97" s="98"/>
+      <c r="C97" s="99"/>
+      <c r="D97" s="100"/>
+      <c r="E97" s="101"/>
+      <c r="F97" s="102"/>
+      <c r="G97" s="103"/>
+      <c r="H97" s="104"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="105"/>
+      <c r="B98" s="106"/>
+      <c r="C98" s="107"/>
+      <c r="D98" s="108"/>
+      <c r="E98" s="109"/>
+      <c r="F98" s="110"/>
+      <c r="G98" s="111"/>
+      <c r="H98" s="112"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="113"/>
+      <c r="B99" s="114"/>
+      <c r="C99" s="115"/>
+      <c r="D99" s="116"/>
+      <c r="E99" s="117"/>
+      <c r="F99" s="118"/>
+      <c r="G99" s="119"/>
+      <c r="H99" s="120"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="121"/>
+      <c r="B100" s="122"/>
+      <c r="C100" s="123"/>
+      <c r="D100" s="124"/>
+      <c r="E100" s="125"/>
+      <c r="F100" s="126"/>
+      <c r="G100" s="127"/>
+      <c r="H100" s="128"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="129"/>
+      <c r="B101" s="130"/>
+      <c r="C101" s="131"/>
+      <c r="D101" s="132"/>
+      <c r="E101" s="133"/>
+      <c r="F101" s="134"/>
+      <c r="G101" s="135"/>
+      <c r="H101" s="136"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="137"/>
+      <c r="B102" s="138"/>
+      <c r="C102" s="139"/>
+      <c r="D102" s="140"/>
+      <c r="E102" s="141"/>
+      <c r="F102" s="142"/>
+      <c r="G102" s="143"/>
+      <c r="H102" s="144"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="145"/>
+      <c r="B103" s="146"/>
+      <c r="C103" s="147"/>
+      <c r="D103" s="148"/>
+      <c r="E103" s="149"/>
+      <c r="F103" s="150"/>
+      <c r="G103" s="151"/>
+      <c r="H103" s="152"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="153"/>
+      <c r="B104" s="154"/>
+      <c r="C104" s="155"/>
+      <c r="D104" s="156"/>
+      <c r="E104" s="157"/>
+      <c r="F104" s="158"/>
+      <c r="G104" s="159"/>
+      <c r="H104" s="160"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>